<commit_message>
Actualización carga de mediciones (Funcionando)
</commit_message>
<xml_diff>
--- a/MedicionesOrganizacion.xlsx
+++ b/MedicionesOrganizacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bntor\Downloads\FACULTAD\2-DISEÑO DE SISTEMAS\DDS-2022-K3002-Grupo_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Desktop\Facultad\UTN3ro\Diseño de sistemas\TP Grupal\DDS-2022-K3002-Grupo_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BC24B7-8021-403B-9AEE-C3E3758DD529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7933DB9-2BB2-4ECD-831B-45A8632EFA7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="1584" windowWidth="17280" windowHeight="8964" xr2:uid="{28E2D1D0-2670-43C5-BE59-E79AAE77875E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{28E2D1D0-2670-43C5-BE59-E79AAE77875E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>valor</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>Consumo</t>
+  </si>
+  <si>
+    <t>50.0</t>
+  </si>
+  <si>
+    <t>30.0</t>
+  </si>
+  <si>
+    <t>10.0</t>
   </si>
 </sst>
 </file>
@@ -122,16 +131,16 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -452,51 +461,51 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
-        <v>50</v>
+      <c r="C3" t="s">
+        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -505,15 +514,15 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
-        <v>30</v>
+      <c r="C4" t="s">
+        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -522,15 +531,15 @@
         <v>44682</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
-        <v>10</v>
+      <c r="C5" t="s">
+        <v>15</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>

</xml_diff>